<commit_message>
Renamed folder again and updated spreadsheets.
</commit_message>
<xml_diff>
--- a/FetchIcons.xlsx
+++ b/FetchIcons.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Mario</t>
   </si>
@@ -284,13 +284,16 @@
   </si>
   <si>
     <t>MiiSwordsman</t>
+  </si>
+  <si>
+    <t>MiiFighter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -310,6 +313,11 @@
       <sz val="9.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -332,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -356,6 +364,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f t="shared" ref="B2:I2" si="1">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A2,"/",$A2,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B2:I2" si="1">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A2,"/",$A2,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C2" s="1" t="str">
@@ -649,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f t="shared" ref="B3:I3" si="2">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A3,"/",$A3,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B3:I3" si="2">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A3,"/",$A3,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C3" s="1" t="str">
@@ -690,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f t="shared" ref="B4:I4" si="4">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A4,"/",$A4,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B4:I4" si="4">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A4,"/",$A4,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C4" s="1" t="str">
@@ -731,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="str">
-        <f t="shared" ref="B5:I5" si="5">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A5,"/",$A5,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B5:I5" si="5">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A5,"/",$A5,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C5" s="1" t="str">
@@ -772,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="str">
-        <f t="shared" ref="B6:I6" si="6">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A6,"/",$A6,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B6:I6" si="6">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A6,"/",$A6,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C6" s="1" t="str">
@@ -813,7 +824,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="str">
-        <f t="shared" ref="B7:I7" si="7">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A7,"/",$A7,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B7:I7" si="7">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A7,"/",$A7,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C7" s="1" t="str">
@@ -854,7 +865,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="str">
-        <f t="shared" ref="B8:I8" si="8">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A8,"/",$A8,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B8:I8" si="8">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A8,"/",$A8,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C8" s="1" t="str">
@@ -895,7 +906,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="str">
-        <f t="shared" ref="B9:I9" si="9">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A9,"/",$A9,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B9:I9" si="9">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A9,"/",$A9,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C9" s="1" t="str">
@@ -936,7 +947,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="str">
-        <f t="shared" ref="B10:I10" si="10">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A10,"/",$A10,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B10:I10" si="10">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A10,"/",$A10,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C10" s="1" t="str">
@@ -977,7 +988,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="str">
-        <f t="shared" ref="B11:I11" si="11">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A11,"/",$A11,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B11:I11" si="11">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A11,"/",$A11,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C11" s="1" t="str">
@@ -1018,7 +1029,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="str">
-        <f t="shared" ref="B12:I12" si="12">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A12,"/",$A12,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B12:I12" si="12">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A12,"/",$A12,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C12" s="1" t="str">
@@ -1059,7 +1070,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="str">
-        <f t="shared" ref="B13:I13" si="13">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A13,"/",$A13,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B13:I13" si="13">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A13,"/",$A13,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C13" s="1" t="str">
@@ -1100,7 +1111,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="str">
-        <f t="shared" ref="B14:I14" si="14">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A14,"/",$A14,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B14:I14" si="14">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A14,"/",$A14,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C14" s="1" t="str">
@@ -1141,7 +1152,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f t="shared" ref="B15:I15" si="15">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A15,"/",$A15,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B15:I15" si="15">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A15,"/",$A15,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C15" s="1" t="str">
@@ -1182,7 +1193,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f t="shared" ref="B16:I16" si="16">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A16,"/",$A16,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B16:I16" si="16">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A16,"/",$A16,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C16" s="1" t="str">
@@ -1223,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="str">
-        <f t="shared" ref="B17:I17" si="17">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A17,"/",$A17,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B17:I17" si="17">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A17,"/",$A17,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C17" s="1" t="str">
@@ -1264,7 +1275,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" ref="B18:I18" si="18">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A18,"/",$A18,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B18:I18" si="18">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A18,"/",$A18,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C18" s="1" t="str">
@@ -1305,7 +1316,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="str">
-        <f t="shared" ref="B19:I19" si="19">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A19,"/",$A19,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B19:I19" si="19">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A19,"/",$A19,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C19" s="1" t="str">
@@ -1346,7 +1357,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="str">
-        <f t="shared" ref="B20:I20" si="20">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A20,"/",$A20,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B20:I20" si="20">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A20,"/",$A20,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C20" s="1" t="str">
@@ -1387,7 +1398,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="str">
-        <f t="shared" ref="B21:I21" si="21">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A21,"/",$A21,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B21:I21" si="21">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A21,"/",$A21,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C21" s="1" t="str">
@@ -1428,7 +1439,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="str">
-        <f t="shared" ref="B22:I22" si="22">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A22,"/",$A22,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B22:I22" si="22">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A22,"/",$A22,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C22" s="1" t="str">
@@ -1469,7 +1480,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="str">
-        <f t="shared" ref="B23:I23" si="23">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A23,"/",$A23,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B23:I23" si="23">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A23,"/",$A23,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C23" s="1" t="str">
@@ -1510,7 +1521,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="str">
-        <f t="shared" ref="B24:I24" si="24">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A24,"/",$A24,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B24:I24" si="24">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A24,"/",$A24,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C24" s="1" t="str">
@@ -1551,7 +1562,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="str">
-        <f t="shared" ref="B25:I25" si="25">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A25,"/",$A25,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B25:I25" si="25">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A25,"/",$A25,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C25" s="1" t="str">
@@ -1592,7 +1603,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="str">
-        <f t="shared" ref="B26:I26" si="26">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A26,"/",$A26,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B26:I26" si="26">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A26,"/",$A26,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C26" s="1" t="str">
@@ -1633,7 +1644,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="str">
-        <f t="shared" ref="B27:I27" si="27">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A27,"/",$A27,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B27:I27" si="27">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A27,"/",$A27,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C27" s="1" t="str">
@@ -1674,7 +1685,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="str">
-        <f t="shared" ref="B28:I28" si="28">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A28,"/",$A28,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B28:I28" si="28">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A28,"/",$A28,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C28" s="1" t="str">
@@ -1715,7 +1726,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="str">
-        <f t="shared" ref="B29:I29" si="29">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A29,"/",$A29,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B29:I29" si="29">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A29,"/",$A29,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C29" s="1" t="str">
@@ -1756,7 +1767,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="str">
-        <f t="shared" ref="B30:I30" si="30">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A30,"/",$A30,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B30:I30" si="30">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A30,"/",$A30,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C30" s="1" t="str">
@@ -1797,7 +1808,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="str">
-        <f t="shared" ref="B31:I31" si="31">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A31,"/",$A31,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B31:I31" si="31">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A31,"/",$A31,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C31" s="1" t="str">
@@ -1838,7 +1849,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="str">
-        <f t="shared" ref="B32:I32" si="32">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A32,"/",$A32,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B32:I32" si="32">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A32,"/",$A32,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C32" s="1" t="str">
@@ -1879,7 +1890,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="str">
-        <f t="shared" ref="B33:I33" si="33">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A33,"/",$A33,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B33:I33" si="33">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A33,"/",$A33,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C33" s="1" t="str">
@@ -1920,7 +1931,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="str">
-        <f t="shared" ref="B34:I34" si="35">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A34,"/",$A34,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B34:I34" si="35">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A34,"/",$A34,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C34" s="1" t="str">
@@ -1961,7 +1972,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="str">
-        <f t="shared" ref="B35:I35" si="36">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A35,"/",$A35,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B35:I35" si="36">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A35,"/",$A35,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C35" s="1" t="str">
@@ -2002,7 +2013,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="str">
-        <f t="shared" ref="B36:I36" si="37">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A36,"/",$A36,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B36:I36" si="37">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A36,"/",$A36,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C36" s="1" t="str">
@@ -2043,7 +2054,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="str">
-        <f t="shared" ref="B37:I37" si="38">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A37,"/",$A37,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B37:I37" si="38">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A37,"/",$A37,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C37" s="1" t="str">
@@ -2084,7 +2095,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="str">
-        <f t="shared" ref="B38:I38" si="39">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A38,"/",$A38,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B38:I38" si="39">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A38,"/",$A38,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C38" s="1" t="str">
@@ -2125,7 +2136,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="str">
-        <f t="shared" ref="B39:I39" si="40">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A39,"/",$A39,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B39:I39" si="40">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A39,"/",$A39,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C39" s="1" t="str">
@@ -2166,7 +2177,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="str">
-        <f t="shared" ref="B40:I40" si="41">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A40,"/",$A40,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B40:I40" si="41">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A40,"/",$A40,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C40" s="1" t="str">
@@ -2207,7 +2218,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="str">
-        <f t="shared" ref="B41:I41" si="42">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A41,"/",$A41,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B41:I41" si="42">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A41,"/",$A41,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C41" s="1" t="str">
@@ -2248,7 +2259,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="str">
-        <f t="shared" ref="B42:I42" si="43">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A42,"/",$A42,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B42:I42" si="43">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A42,"/",$A42,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C42" s="1" t="str">
@@ -2289,7 +2300,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="str">
-        <f t="shared" ref="B43:I43" si="44">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A43,"/",$A43,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B43:I43" si="44">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A43,"/",$A43,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C43" s="1" t="str">
@@ -2330,7 +2341,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="str">
-        <f t="shared" ref="B44:I44" si="45">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A44,"/",$A44,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B44:I44" si="45">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A44,"/",$A44,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C44" s="1" t="str">
@@ -2371,7 +2382,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="str">
-        <f t="shared" ref="B45:I45" si="46">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A45,"/",$A45,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B45:I45" si="46">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A45,"/",$A45,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C45" s="1" t="str">
@@ -2412,7 +2423,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="str">
-        <f t="shared" ref="B46:I46" si="47">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A46,"/",$A46,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B46:I46" si="47">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A46,"/",$A46,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C46" s="1" t="str">
@@ -2453,7 +2464,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="str">
-        <f t="shared" ref="B47:I47" si="48">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A47,"/",$A47,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B47:I47" si="48">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A47,"/",$A47,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C47" s="1" t="str">
@@ -2494,7 +2505,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="str">
-        <f t="shared" ref="B48:I48" si="49">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A48,"/",$A48,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B48:I48" si="49">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A48,"/",$A48,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C48" s="1" t="str">
@@ -2535,7 +2546,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="str">
-        <f t="shared" ref="B49:I49" si="50">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A49,"/",$A49,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B49:I49" si="50">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A49,"/",$A49,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C49" s="1" t="str">
@@ -2576,7 +2587,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="str">
-        <f t="shared" ref="B50:I50" si="51">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A50,"/",$A50,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B50:I50" si="51">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A50,"/",$A50,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C50" s="1" t="str">
@@ -2617,7 +2628,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="str">
-        <f t="shared" ref="B51:I51" si="52">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A51,"/",$A51,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B51:I51" si="52">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A51,"/",$A51,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C51" s="1" t="str">
@@ -2658,7 +2669,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="str">
-        <f t="shared" ref="B52:I52" si="53">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A52,"/",$A52,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B52:I52" si="53">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A52,"/",$A52,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C52" s="1" t="str">
@@ -2699,7 +2710,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="str">
-        <f t="shared" ref="B53:I53" si="54">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A53,"/",$A53,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B53:I53" si="54">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A53,"/",$A53,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C53" s="1" t="str">
@@ -2740,7 +2751,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="str">
-        <f t="shared" ref="B54:I54" si="55">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A54,"/",$A54,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B54:I54" si="55">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A54,"/",$A54,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C54" s="1" t="str">
@@ -2781,7 +2792,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="str">
-        <f t="shared" ref="B55:I55" si="56">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A55,"/",$A55,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B55:I55" si="56">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A55,"/",$A55,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C55" s="1" t="str">
@@ -2822,7 +2833,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="str">
-        <f t="shared" ref="B56:I56" si="57">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A56,"/",$A56,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B56:I56" si="57">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A56,"/",$A56,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C56" s="1" t="str">
@@ -2863,7 +2874,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="str">
-        <f t="shared" ref="B57:I57" si="58">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A57,"/",$A57,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B57:I57" si="58">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A57,"/",$A57,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C57" s="1" t="str">
@@ -2904,7 +2915,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="str">
-        <f t="shared" ref="B58:I58" si="59">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A58,"/",$A58,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B58:I58" si="59">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A58,"/",$A58,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C58" s="1" t="str">
@@ -2945,7 +2956,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="1" t="str">
-        <f t="shared" ref="B59:I59" si="60">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A59,"/",$A59,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B59:I59" si="60">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A59,"/",$A59,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C59" s="1" t="str">
@@ -2986,7 +2997,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="1" t="str">
-        <f t="shared" ref="B60:I60" si="61">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A60,"/",$A60,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B60:I60" si="61">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A60,"/",$A60,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C60" s="1" t="str">
@@ -3027,7 +3038,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="1" t="str">
-        <f t="shared" ref="B61:I61" si="62">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A61,"/",$A61,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B61:I61" si="62">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A61,"/",$A61,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C61" s="1" t="str">
@@ -3068,7 +3079,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="str">
-        <f t="shared" ref="B62:I62" si="63">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A62,"/",$A62,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B62:I62" si="63">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A62,"/",$A62,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C62" s="1" t="str">
@@ -3109,7 +3120,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="1" t="str">
-        <f t="shared" ref="B63:I63" si="64">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A63,"/",$A63,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B63:I63" si="64">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A63,"/",$A63,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C63" s="1" t="str">
@@ -3150,7 +3161,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="1" t="str">
-        <f t="shared" ref="B64:I64" si="65">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A64,"/",$A64,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B64:I64" si="65">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A64,"/",$A64,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C64" s="1" t="str">
@@ -3191,7 +3202,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="1" t="str">
-        <f t="shared" ref="B65:I65" si="66">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A65,"/",$A65,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B65:I65" si="66">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A65,"/",$A65,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C65" s="1" t="str">
@@ -3232,7 +3243,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="1" t="str">
-        <f t="shared" ref="B66:I66" si="67">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A66,"/",$A66,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B66:I66" si="67">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A66,"/",$A66,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C66" s="1" t="str">
@@ -3273,7 +3284,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="1" t="str">
-        <f t="shared" ref="B67:I67" si="68">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A67,"/",$A67,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B67:I67" si="68">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A67,"/",$A67,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C67" s="1" t="str">
@@ -3314,7 +3325,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="1" t="str">
-        <f t="shared" ref="B68:I68" si="69">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A68,"/",$A68,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B68:I68" si="69">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A68,"/",$A68,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C68" s="1" t="str">
@@ -3355,7 +3366,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="1" t="str">
-        <f t="shared" ref="B69:I69" si="71">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A69,"/",$A69,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B69:I69" si="71">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A69,"/",$A69,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C69" s="1" t="str">
@@ -3396,7 +3407,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="1" t="str">
-        <f t="shared" ref="B70:I70" si="72">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A70,"/",$A70,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B70:I70" si="72">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A70,"/",$A70,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C70" s="1" t="str">
@@ -3437,7 +3448,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="1" t="str">
-        <f t="shared" ref="B71:I71" si="73">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A71,"/",$A71,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B71:I71" si="73">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A71,"/",$A71,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C71" s="1" t="str">
@@ -3478,7 +3489,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="str">
-        <f t="shared" ref="B72:I72" si="74">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A72,"/",$A72,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B72:I72" si="74">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A72,"/",$A72,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C72" s="1" t="str">
@@ -3519,7 +3530,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="1" t="str">
-        <f t="shared" ref="B73:I73" si="75">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A73,"/",$A73,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B73:I73" si="75">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A73,"/",$A73,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C73" s="1" t="str">
@@ -3560,7 +3571,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="1" t="str">
-        <f t="shared" ref="B74:I74" si="76">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A74,"/",$A74,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B74:I74" si="76">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A74,"/",$A74,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C74" s="1" t="str">
@@ -3601,7 +3612,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="str">
-        <f t="shared" ref="B75:I75" si="77">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A75,"/",$A75,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B75:I75" si="77">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A75,"/",$A75,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C75" s="1" t="str">
@@ -3642,7 +3653,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="str">
-        <f t="shared" ref="B76:I76" si="78">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A76,"/",$A76,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B76:I76" si="78">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A76,"/",$A76,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C76" s="1" t="str">
@@ -3683,7 +3694,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="1" t="str">
-        <f t="shared" ref="B77:I77" si="79">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A77,"/",$A77,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B77:I77" si="79">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A77,"/",$A77,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C77" s="1" t="str">
@@ -3724,7 +3735,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="1" t="str">
-        <f t="shared" ref="B78:I78" si="80">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A78,"/",$A78,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B78:I78" si="80">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A78,"/",$A78,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C78" s="1" t="str">
@@ -3765,7 +3776,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="str">
-        <f t="shared" ref="B79:I79" si="81">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A79,"/",$A79,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B79:I79" si="81">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A79,"/",$A79,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C79" s="1" t="str">
@@ -3806,7 +3817,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="1" t="str">
-        <f t="shared" ref="B80:I80" si="82">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A80,"/",$A80,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B80:I80" si="82">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A80,"/",$A80,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C80" s="1" t="str">
@@ -3847,7 +3858,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="1" t="str">
-        <f t="shared" ref="B81:I81" si="83">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A81,"/",$A81,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B81:I81" si="83">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A81,"/",$A81,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C81" s="1" t="str">
@@ -3888,7 +3899,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="1" t="str">
-        <f t="shared" ref="B82:I82" si="84">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A82,"/",$A82,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B82:I82" si="84">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A82,"/",$A82,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C82" s="1" t="str">
@@ -3929,7 +3940,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="1" t="str">
-        <f t="shared" ref="B83:I83" si="85">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A83,"/",$A83,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B83:I83" si="85">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A83,"/",$A83,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C83" s="1" t="str">
@@ -3970,7 +3981,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="1" t="str">
-        <f t="shared" ref="B84:I84" si="86">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A84,"/",$A84,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B84:I84" si="86">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A84,"/",$A84,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C84" s="1" t="str">
@@ -4011,7 +4022,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="1" t="str">
-        <f t="shared" ref="B85:I85" si="87">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A85,"/",$A85,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B85:I85" si="87">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A85,"/",$A85,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C85" s="1" t="str">
@@ -4052,7 +4063,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="str">
-        <f t="shared" ref="B86:I86" si="88">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A86,"/",$A86,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B86:I86" si="88">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A86,"/",$A86,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C86" s="1" t="str">
@@ -4093,7 +4104,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="1" t="str">
-        <f t="shared" ref="B87:I87" si="89">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A87,"/",$A87,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B87:I87" si="89">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A87,"/",$A87,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C87" s="1" t="str">
@@ -4134,7 +4145,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="1" t="str">
-        <f t="shared" ref="B88:I88" si="90">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A88,"/",$A88,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B88:I88" si="90">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A88,"/",$A88,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C88" s="1" t="str">
@@ -4175,7 +4186,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="1" t="str">
-        <f t="shared" ref="B89:I89" si="91">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A89,"/",$A89,B$1,".png?=version2"))</f>
+        <f t="shared" ref="B89:I89" si="91">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A89,"/",$A89,B$1,".png?=version3"))</f>
         <v/>
       </c>
       <c r="C89" s="1" t="str">
@@ -4216,7 +4227,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="1" t="str">
-        <f t="shared" ref="B90:B92" si="92">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A90,"/",$A90,".png?version=1"))</f>
+        <f t="shared" ref="B90:B93" si="92">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A90,"/",$A90,".png?version=1"))</f>
         <v/>
       </c>
       <c r="C90" s="7"/>
@@ -4227,7 +4238,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1" t="str">
-        <f t="shared" ref="J90:J92" si="93">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A90,"/",$A90,".png?version=1"))</f>
+        <f t="shared" ref="J90:J93" si="93">IMAGE(CONCATENATE("https://raw.githubusercontent.com/goingtodq/ssbu-character-icons/refs/heads/main/icons/",$A90,"/",$A90,".png?version=1"))</f>
         <v/>
       </c>
     </row>
@@ -4271,6 +4282,19 @@
         <v/>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" s="1" t="str">
+        <f t="shared" si="92"/>
+        <v/>
+      </c>
+      <c r="J93" s="1" t="str">
+        <f t="shared" si="93"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>